<commit_message>
updated timesheet template file
</commit_message>
<xml_diff>
--- a/app/assets/timesheet_template.xlsx
+++ b/app/assets/timesheet_template.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0" showHorizontalScroll="1" showVerticalScroll="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Template" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
   <extLst>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">First Last
 Position: N/A</t>
@@ -46,6 +46,9 @@
   <si>
     <t xml:space="preserve">Total Hours: N/A</t>
   </si>
+  <si>
+    <t xml:space="preserve">By signing below, I certify that the hours recorded in this timesheet are true, accurate, and complete to the best of my knowledge:</t>
+  </si>
 </sst>
 </file>
 
@@ -55,7 +58,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="hh:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -64,6 +67,20 @@
     <font>
       <sz val="10.000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11.000000"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -76,16 +93,30 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12.000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -94,8 +125,81 @@
       <diagonal style="none"/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
       <left style="medium">
         <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
       </left>
       <right style="medium">
         <color theme="1"/>
@@ -109,7 +213,7 @@
       <diagonal style="none"/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -118,50 +222,70 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="2" fillId="2" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="3" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf fontId="4" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf fontId="4" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="1" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf fontId="4" fillId="0" borderId="2" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="1" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf fontId="5" fillId="0" borderId="2" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="1" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf fontId="5" fillId="0" borderId="2" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf fontId="5" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="1" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf fontId="4" fillId="0" borderId="3" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="4" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="6" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="6" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="6" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
+    <cellStyle name="Output" xfId="6" builtinId="21"/>
+    <cellStyle name="Explanatory Text" xfId="7" builtinId="53"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -633,7 +757,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="1"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" zoomScale="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" topLeftCell="A3" zoomScale="100" workbookViewId="0">
       <selection activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -837,23 +961,36 @@
       <c r="A16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="9" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="17" ht="52.200000000000003" customHeight="1">
+      <c r="A17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A17:F17"/>
+  </mergeCells>
   <printOptions headings="0" gridLines="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.51181102362204689" footer="0.51181102362204689"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>